<commit_message>
2.xlsx er tilbúið sem áætlun, þarf bara að setja inn í 3.ítrunar möppu
git-svn-id: https://tgapc93.rhi.hi.is/svn/softdev/2013/hopur19@8229 5d233661-44a1-474e-bded-f455fa16cf90
</commit_message>
<xml_diff>
--- a/stada.xlsx
+++ b/stada.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="itrun 1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
   <si>
     <t>Notendasögur</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Vinna úr gögnum</t>
   </si>
   <si>
-    <t>Verkþættir 1 og 2</t>
-  </si>
-  <si>
     <t>Sýnt gröf um fyrirtæki</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>Laga útlit á gröfum</t>
   </si>
   <si>
-    <t>Verkþættir 1,2 og 3</t>
-  </si>
-  <si>
     <t>Ná í vísitölur</t>
   </si>
   <si>
@@ -166,12 +160,6 @@
     <t>Skrifa commandlykkju</t>
   </si>
   <si>
-    <t>Lengd ítrunar</t>
-  </si>
-  <si>
-    <t>Ráðstafaður tími</t>
-  </si>
-  <si>
     <t>Framkvæma tæknigreiningu</t>
   </si>
   <si>
@@ -208,9 +196,6 @@
     <t>Margir gluggar</t>
   </si>
   <si>
-    <t>Kynna sér wxPython</t>
-  </si>
-  <si>
     <t>Búa til gluggaumhverfi</t>
   </si>
   <si>
@@ -235,17 +220,32 @@
     <t>Hjálp við ákvörðunartöku</t>
   </si>
   <si>
-    <t>Forrit sem varar einstakling við ef verð fellur innan marka sem hann hefur sett</t>
-  </si>
-  <si>
-    <t>Forrit sem bendir einstakling á ef fyrirtæki gengur vel</t>
+    <t>Velja hluti í upphafssýn</t>
+  </si>
+  <si>
+    <t>Tengja saman tilbúna glugga</t>
+  </si>
+  <si>
+    <t>Tengja glugga við forrit</t>
+  </si>
+  <si>
+    <t>Tengja glugga v/ forrit</t>
+  </si>
+  <si>
+    <t>Ráðstafaður tími:</t>
+  </si>
+  <si>
+    <t>Lengd ítrunar:</t>
+  </si>
+  <si>
+    <t>Forrit sem segir hvort kaupa eigi eða selja út frá SMA og Beta-stuðli</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -265,6 +265,18 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -447,10 +459,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -554,22 +580,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -584,28 +598,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -620,8 +628,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,7 +711,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Lengd ítrunar</c:v>
+                  <c:v>Lengd ítrunar:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -683,7 +726,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.6</c:v>
+                  <c:v>5.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -713,11 +756,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2092752104"/>
-        <c:axId val="2092873864"/>
+        <c:axId val="2096503896"/>
+        <c:axId val="2096865032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2092752104"/>
+        <c:axId val="2096503896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -727,12 +770,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092873864"/>
+        <c:crossAx val="2096865032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2092873864"/>
+        <c:axId val="2096865032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092752104"/>
+        <c:crossAx val="2096503896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -804,11 +847,16 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Lengd ítrunar</c:v>
+                  <c:v>Lengd ítrunar:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'Ítrun 2'!$N$4:$O$4</c:f>
@@ -849,11 +897,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2092542216"/>
-        <c:axId val="2092708232"/>
+        <c:axId val="2096618904"/>
+        <c:axId val="2096522088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2092542216"/>
+        <c:axId val="2096618904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,12 +911,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092708232"/>
+        <c:crossAx val="2096522088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2092708232"/>
+        <c:axId val="2096522088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -878,11 +926,125 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092542216"/>
+        <c:crossAx val="2096618904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ítrun 3'!$N$4:$O$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ítrun 3'!$N$5:$O$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2088735768"/>
+        <c:axId val="2088738728"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2088735768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2088738728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2088738728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2088735768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -906,7 +1068,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2184400</xdr:colOff>
+      <xdr:colOff>2057400</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -935,19 +1097,54 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
+      <xdr:colOff>406400</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>2336800</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2108200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>336550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>298450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1290,7 +1487,7 @@
   <dimension ref="A3:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="M4" sqref="M4:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1308,7 +1505,9 @@
     <col min="11" max="11" width="29.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14" max="19" width="10.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7" style="1" customWidth="1"/>
+    <col min="16" max="19" width="10.33203125" style="1" customWidth="1"/>
     <col min="20" max="16384" width="17.1640625" style="1"/>
   </cols>
   <sheetData>
@@ -1316,43 +1515,43 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="12">
       <c r="A4" s="3"/>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="42" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="42" t="s">
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>5.6</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="12">
@@ -1360,20 +1559,20 @@
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="38"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="41"/>
       <c r="L5" s="5"/>
       <c r="M5" s="1" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="N5" s="1">
         <v>4.3</v>
@@ -1392,12 +1591,12 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="39"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="42"/>
       <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:15" ht="51" customHeight="1">
@@ -1410,14 +1609,12 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="36"/>
-      <c r="K7" s="39"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="42"/>
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:15" ht="12">
@@ -1426,12 +1623,12 @@
       <c r="C8" s="2"/>
       <c r="D8" s="10"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="40"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="43"/>
       <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:15" ht="12">
@@ -1439,18 +1636,18 @@
       <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="L9" s="5"/>
     </row>
@@ -1463,36 +1660,34 @@
         <v>7</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
       <c r="K10" s="12"/>
       <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:15" ht="48">
       <c r="A11" s="3"/>
       <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
       <c r="K11" s="13"/>
       <c r="L11" s="5"/>
     </row>
@@ -1502,11 +1697,11 @@
       <c r="C12" s="2"/>
       <c r="D12" s="10"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
       <c r="K12" s="13"/>
       <c r="L12" s="5"/>
     </row>
@@ -1515,16 +1710,16 @@
       <c r="B13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="35"/>
+      <c r="C13" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="36"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
       <c r="K13" s="13"/>
       <c r="L13" s="5"/>
     </row>
@@ -1538,33 +1733,31 @@
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
       <c r="K14" s="14"/>
       <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:15" ht="24">
       <c r="A15" s="3"/>
       <c r="B15" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
       <c r="K15" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L15" s="5"/>
     </row>
@@ -1574,11 +1767,11 @@
       <c r="C16" s="2"/>
       <c r="D16" s="10"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
       <c r="K16" s="12" t="s">
         <v>5</v>
       </c>
@@ -1589,18 +1782,18 @@
       <c r="B17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="35"/>
+      <c r="C17" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="36"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
       <c r="K17" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L17" s="5"/>
     </row>
@@ -1614,35 +1807,33 @@
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
       <c r="K18" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="36">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
       <c r="K19" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L19" s="5"/>
     </row>
@@ -1652,11 +1843,11 @@
       <c r="C20" s="2"/>
       <c r="D20" s="10"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
       <c r="K20" s="13"/>
       <c r="L20" s="5"/>
     </row>
@@ -1665,20 +1856,20 @@
       <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="35"/>
+      <c r="C21" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="36"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
       <c r="K21" s="13"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="24">
+    <row r="22" spans="1:12" ht="12">
       <c r="A22" s="3"/>
       <c r="B22" s="7" t="s">
         <v>6</v>
@@ -1686,29 +1877,27 @@
       <c r="C22" s="8"/>
       <c r="D22" s="11"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
       <c r="K22" s="13"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" ht="24">
       <c r="A23" s="3"/>
       <c r="B23" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="10"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
       <c r="H23" s="9"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
       <c r="K23" s="14"/>
       <c r="L23" s="5"/>
     </row>
@@ -1726,21 +1915,26 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K5:K8"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I17:J17"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="C9:D9"/>
@@ -1755,26 +1949,21 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K5:K8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1793,8 +1982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1820,37 +2009,37 @@
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
       <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:15" ht="12">
       <c r="A4" s="17"/>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="54" t="s">
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="55"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="54" t="s">
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
       <c r="K4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="18" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N4" s="18">
         <v>0</v>
@@ -1864,20 +2053,20 @@
       <c r="B5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="49"/>
+      <c r="C5" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="46"/>
       <c r="E5" s="22"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="22"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="50"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="51"/>
       <c r="L5" s="21"/>
       <c r="M5" s="18" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="N5" s="18">
         <v>5</v>
@@ -1895,35 +2084,35 @@
         <v>7</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="21"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="51"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="21"/>
     </row>
     <row r="7" spans="1:15" ht="60" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E7" s="21"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="51"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="52"/>
       <c r="L7" s="21"/>
     </row>
     <row r="8" spans="1:15" ht="12">
@@ -1932,12 +2121,12 @@
       <c r="C8" s="19"/>
       <c r="D8" s="26"/>
       <c r="E8" s="25"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
       <c r="H8" s="25"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="52"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="53"/>
       <c r="L8" s="21"/>
     </row>
     <row r="9" spans="1:15" ht="12">
@@ -1945,18 +2134,18 @@
       <c r="B9" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="49"/>
+      <c r="C9" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="46"/>
       <c r="E9" s="22"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="22"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
       <c r="K9" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L9" s="21"/>
     </row>
@@ -1969,34 +2158,34 @@
         <v>7</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="21"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
       <c r="H10" s="21"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
       <c r="K10" s="28"/>
       <c r="L10" s="21"/>
     </row>
     <row r="11" spans="1:15" ht="48">
       <c r="A11" s="17"/>
       <c r="B11" s="21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E11" s="21"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
       <c r="K11" s="29"/>
       <c r="L11" s="21"/>
     </row>
@@ -2006,11 +2195,11 @@
       <c r="C12" s="19"/>
       <c r="D12" s="26"/>
       <c r="E12" s="25"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
       <c r="K12" s="29"/>
       <c r="L12" s="21"/>
     </row>
@@ -2019,13 +2208,13 @@
       <c r="B13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="49"/>
+      <c r="C13" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="46"/>
       <c r="E13" s="22"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
       <c r="H13" s="22"/>
       <c r="I13" s="31"/>
       <c r="J13" s="32"/>
@@ -2042,31 +2231,26 @@
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="21"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="21"/>
       <c r="J14" s="17"/>
       <c r="K14" s="33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:15" ht="48">
+    <row r="15" spans="1:15" ht="36">
       <c r="A15" s="17"/>
       <c r="B15" s="21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>31</v>
-      </c>
+      <c r="G15" s="17"/>
       <c r="H15" s="21"/>
       <c r="J15" s="34"/>
       <c r="K15" s="33"/>
@@ -2078,29 +2262,29 @@
       <c r="C16" s="19"/>
       <c r="D16" s="26"/>
       <c r="E16" s="25"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
       <c r="H16" s="25"/>
       <c r="I16" s="19"/>
       <c r="J16" s="26"/>
       <c r="K16" s="29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L16" s="21"/>
     </row>
     <row r="17" spans="1:12" ht="12">
       <c r="A17" s="17"/>
       <c r="B17" s="22"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="22"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="22"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
       <c r="K17" s="29" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L17" s="21"/>
     </row>
@@ -2110,12 +2294,14 @@
       <c r="C18" s="24"/>
       <c r="D18" s="27"/>
       <c r="E18" s="21"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
       <c r="H18" s="21"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="29"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="29" t="s">
+        <v>29</v>
+      </c>
       <c r="L18" s="21"/>
     </row>
     <row r="19" spans="1:12" ht="12">
@@ -2123,11 +2309,11 @@
       <c r="B19" s="21"/>
       <c r="D19" s="17"/>
       <c r="E19" s="21"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
       <c r="H19" s="21"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
       <c r="K19" s="29"/>
       <c r="L19" s="21"/>
     </row>
@@ -2137,43 +2323,79 @@
       <c r="C20" s="19"/>
       <c r="D20" s="26"/>
       <c r="E20" s="25"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
       <c r="H20" s="25"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
       <c r="K20" s="30"/>
       <c r="L20" s="21"/>
     </row>
     <row r="21" spans="1:12" ht="12">
       <c r="B21" s="31"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="31"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
       <c r="H21" s="31"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
       <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:12" ht="12">
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
     </row>
     <row r="23" spans="1:12" ht="12.75" customHeight="1">
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K5:K8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="I5:J5"/>
@@ -2182,42 +2404,6 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K5:K8"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2232,10 +2418,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L23"/>
+  <dimension ref="A3:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2249,63 +2435,86 @@
     <col min="9" max="9" width="17.1640625" style="18"/>
     <col min="10" max="10" width="10.33203125" style="18" customWidth="1"/>
     <col min="11" max="11" width="36.5" style="18" customWidth="1"/>
-    <col min="12" max="19" width="10.33203125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="14.5" style="18" customWidth="1"/>
+    <col min="14" max="15" width="7.33203125" style="18" customWidth="1"/>
+    <col min="16" max="19" width="10.33203125" style="18" customWidth="1"/>
     <col min="20" max="16384" width="17.1640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="12">
+    <row r="3" spans="1:15" ht="12">
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
       <c r="K3" s="19"/>
     </row>
-    <row r="4" spans="1:12" ht="12">
+    <row r="4" spans="1:15" ht="12">
       <c r="A4" s="17"/>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="54" t="s">
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="55"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="54" t="s">
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
       <c r="K4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="L4" s="21"/>
-    </row>
-    <row r="5" spans="1:12" ht="12">
+      <c r="M4" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="35">
+        <v>0</v>
+      </c>
+      <c r="O4" s="35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="12">
       <c r="A5" s="17"/>
       <c r="B5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="49"/>
+      <c r="C5" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="46"/>
       <c r="E5" s="22"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="F5" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="46"/>
       <c r="H5" s="22"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="50"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="51"/>
       <c r="L5" s="21"/>
-    </row>
-    <row r="6" spans="1:12" ht="12">
+      <c r="M5" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" s="35">
+        <v>9</v>
+      </c>
+      <c r="O5" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="12">
       <c r="A6" s="17"/>
       <c r="B6" s="23" t="s">
         <v>6</v>
@@ -2315,67 +2524,71 @@
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="21"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
+      <c r="F6" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="54"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="51"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="21"/>
     </row>
-    <row r="7" spans="1:12" ht="51" customHeight="1">
+    <row r="7" spans="1:15" ht="51" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="17"/>
+        <v>47</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="E7" s="21"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="51"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="52"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="1:12" ht="12">
+    <row r="8" spans="1:15" ht="12">
       <c r="A8" s="17"/>
       <c r="B8" s="25"/>
       <c r="C8" s="19"/>
       <c r="D8" s="26"/>
       <c r="E8" s="25"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
       <c r="H8" s="25"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="52"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="53"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:12" ht="12">
+    <row r="9" spans="1:15" ht="12">
       <c r="A9" s="17"/>
       <c r="B9" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="49"/>
+      <c r="C9" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="46"/>
       <c r="E9" s="22"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="22"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
       <c r="K9" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:12" ht="12">
+    <row r="10" spans="1:15" ht="12">
       <c r="A10" s="17"/>
       <c r="B10" s="23" t="s">
         <v>6</v>
@@ -2385,65 +2598,65 @@
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
       <c r="H10" s="21"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
       <c r="K10" s="28"/>
       <c r="L10" s="21"/>
     </row>
-    <row r="11" spans="1:12" ht="36">
+    <row r="11" spans="1:15" ht="36">
       <c r="A11" s="17"/>
       <c r="B11" s="21" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="21"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
       <c r="K11" s="29"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:12" ht="12">
+    <row r="12" spans="1:15" ht="12">
       <c r="A12" s="17"/>
       <c r="B12" s="25"/>
       <c r="C12" s="19"/>
       <c r="D12" s="26"/>
       <c r="E12" s="25"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
       <c r="K12" s="29"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="12">
+    <row r="13" spans="1:15" ht="12">
       <c r="A13" s="17"/>
       <c r="B13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="49"/>
+      <c r="C13" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="46"/>
       <c r="E13" s="22"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
       <c r="H13" s="22"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
       <c r="K13" s="29"/>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:12" ht="12">
+    <row r="14" spans="1:15" ht="12">
       <c r="A14" s="17"/>
       <c r="B14" s="23" t="s">
         <v>6</v>
@@ -2452,51 +2665,55 @@
         <v>7</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="21"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="21"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
       <c r="K14" s="30"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:12" ht="24">
+    <row r="15" spans="1:15" ht="24">
       <c r="A15" s="17"/>
       <c r="B15" s="21" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="47"/>
+      <c r="F15" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="54"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
+      <c r="I15" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="54"/>
       <c r="K15" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L15" s="21"/>
     </row>
-    <row r="16" spans="1:12" ht="12">
+    <row r="16" spans="1:15" ht="12">
       <c r="A16" s="17"/>
       <c r="B16" s="25"/>
       <c r="C16" s="19"/>
       <c r="D16" s="26"/>
       <c r="E16" s="25"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
       <c r="H16" s="25"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="28"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="L16" s="21"/>
     </row>
     <row r="17" spans="1:12" ht="12">
@@ -2504,16 +2721,16 @@
       <c r="B17" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="49"/>
+      <c r="C17" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="46"/>
       <c r="E17" s="22"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="22"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
       <c r="K17" s="29"/>
       <c r="L17" s="21"/>
     </row>
@@ -2527,29 +2744,28 @@
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="21"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
       <c r="H18" s="21"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
       <c r="K18" s="29"/>
       <c r="L18" s="21"/>
     </row>
-    <row r="19" spans="1:12" ht="60">
+    <row r="19" spans="1:12" ht="48">
       <c r="A19" s="17"/>
       <c r="B19" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="21"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
+      <c r="F19" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="54"/>
       <c r="H19" s="21"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
       <c r="K19" s="29"/>
       <c r="L19" s="21"/>
     </row>
@@ -2559,70 +2775,55 @@
       <c r="C20" s="19"/>
       <c r="D20" s="26"/>
       <c r="E20" s="25"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
       <c r="H20" s="25"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
       <c r="K20" s="30"/>
       <c r="L20" s="21"/>
     </row>
     <row r="21" spans="1:12" ht="12">
       <c r="B21" s="31"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="31"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
       <c r="H21" s="31"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
       <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:12" ht="12">
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
     </row>
     <row r="23" spans="1:12" ht="12.75" customHeight="1">
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K5:K8"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="I5:J5"/>
@@ -2633,20 +2834,37 @@
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K5:K8"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
stada.xlsx tilbúið en á ekki að skila
git-svn-id: https://tgapc93.rhi.hi.is/svn/softdev/2013/hopur19@8341 5d233661-44a1-474e-bded-f455fa16cf90
</commit_message>
<xml_diff>
--- a/stada.xlsx
+++ b/stada.xlsx
@@ -280,18 +280,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -520,9 +514,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -578,6 +569,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1040,11 +1034,6 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1132,15 +1121,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2108200</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>336550</xdr:rowOff>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>298450</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2197100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1487,7 +1476,7 @@
   <dimension ref="A3:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:O5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1746,7 +1735,7 @@
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="35" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="3"/>
@@ -1902,16 +1891,16 @@
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" ht="12">
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="49">
@@ -1988,37 +1977,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="4" style="18" customWidth="1"/>
-    <col min="6" max="8" width="10.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="18"/>
-    <col min="10" max="10" width="10.33203125" style="18" customWidth="1"/>
-    <col min="11" max="11" width="36.5" style="18" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" style="18" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="18" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" style="18" customWidth="1"/>
-    <col min="15" max="15" width="6" style="18" customWidth="1"/>
-    <col min="16" max="19" width="10.33203125" style="18" customWidth="1"/>
-    <col min="20" max="16384" width="17.1640625" style="18"/>
+    <col min="1" max="1" width="1.6640625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="17" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="4" style="17" customWidth="1"/>
+    <col min="6" max="8" width="10.33203125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="17"/>
+    <col min="10" max="10" width="10.33203125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="36.5" style="17" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="17" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="6" style="17" customWidth="1"/>
+    <col min="16" max="19" width="10.33203125" style="17" customWidth="1"/>
+    <col min="20" max="16384" width="17.1640625" style="17"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:15" ht="12">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="47"/>
       <c r="F3" s="47"/>
       <c r="G3" s="47"/>
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
       <c r="J3" s="47"/>
-      <c r="K3" s="19"/>
+      <c r="K3" s="18"/>
     </row>
     <row r="4" spans="1:15" ht="12">
-      <c r="A4" s="17"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="48" t="s">
         <v>0</v>
       </c>
@@ -2034,319 +2023,319 @@
       </c>
       <c r="I4" s="49"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="18" t="s">
+      <c r="L4" s="20"/>
+      <c r="M4" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="17">
         <v>0</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4" s="17">
         <v>7.14</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="12">
-      <c r="A5" s="17"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="46" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="46"/>
-      <c r="E5" s="22"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="46"/>
       <c r="G5" s="46"/>
-      <c r="H5" s="22"/>
+      <c r="H5" s="21"/>
       <c r="I5" s="46"/>
       <c r="J5" s="46"/>
       <c r="K5" s="51"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="18" t="s">
+      <c r="L5" s="20"/>
+      <c r="M5" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="17">
         <v>5</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="12">
-      <c r="A6" s="17"/>
-      <c r="B6" s="23" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="21"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="54"/>
       <c r="G6" s="54"/>
-      <c r="H6" s="21"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="54"/>
       <c r="J6" s="54"/>
       <c r="K6" s="52"/>
-      <c r="L6" s="21"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:15" ht="60" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="54"/>
       <c r="G7" s="54"/>
-      <c r="H7" s="21"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="54"/>
       <c r="J7" s="54"/>
       <c r="K7" s="52"/>
-      <c r="L7" s="21"/>
+      <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:15" ht="12">
-      <c r="A8" s="17"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="55"/>
       <c r="G8" s="55"/>
-      <c r="H8" s="25"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="55"/>
       <c r="J8" s="55"/>
       <c r="K8" s="53"/>
-      <c r="L8" s="21"/>
+      <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:15" ht="12">
-      <c r="A9" s="17"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="46" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="46"/>
-      <c r="E9" s="22"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="46"/>
       <c r="G9" s="46"/>
-      <c r="H9" s="22"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="46"/>
       <c r="J9" s="46"/>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="21"/>
+      <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:15" ht="12">
-      <c r="A10" s="17"/>
-      <c r="B10" s="23" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="54"/>
       <c r="G10" s="54"/>
-      <c r="H10" s="21"/>
+      <c r="H10" s="20"/>
       <c r="I10" s="54"/>
       <c r="J10" s="54"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="21"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:15" ht="48">
-      <c r="A11" s="17"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="54"/>
       <c r="G11" s="54"/>
-      <c r="H11" s="21"/>
+      <c r="H11" s="20"/>
       <c r="I11" s="54"/>
       <c r="J11" s="54"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="21"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:15" ht="12">
-      <c r="A12" s="17"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="25"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="55"/>
       <c r="G12" s="55"/>
-      <c r="H12" s="25"/>
+      <c r="H12" s="24"/>
       <c r="I12" s="55"/>
       <c r="J12" s="55"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="21"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:15" ht="12">
-      <c r="A13" s="17"/>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="46" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="46"/>
-      <c r="E13" s="22"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="46"/>
       <c r="G13" s="46"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="20"/>
     </row>
     <row r="14" spans="1:15" ht="12">
-      <c r="A14" s="17"/>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="21"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
-      <c r="H14" s="21"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="33" t="s">
+      <c r="H14" s="20"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="21"/>
+      <c r="L14" s="20"/>
     </row>
     <row r="15" spans="1:15" ht="36">
-      <c r="A15" s="17"/>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="21"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="21"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="34"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="20"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="20"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
     </row>
     <row r="16" spans="1:15" ht="12">
-      <c r="A16" s="17"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="25"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="29" t="s">
+      <c r="H16" s="24"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="21"/>
+      <c r="L16" s="20"/>
     </row>
     <row r="17" spans="1:12" ht="12">
-      <c r="A17" s="17"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="46"/>
       <c r="D17" s="46"/>
-      <c r="E17" s="22"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="46"/>
       <c r="G17" s="46"/>
-      <c r="H17" s="22"/>
+      <c r="H17" s="21"/>
       <c r="I17" s="46"/>
       <c r="J17" s="46"/>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="21"/>
+      <c r="L17" s="20"/>
     </row>
     <row r="18" spans="1:12" ht="12">
-      <c r="A18" s="17"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="21"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
-      <c r="H18" s="21"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="54"/>
       <c r="J18" s="54"/>
-      <c r="K18" s="29" t="s">
+      <c r="K18" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="21"/>
+      <c r="L18" s="20"/>
     </row>
     <row r="19" spans="1:12" ht="12">
-      <c r="A19" s="17"/>
-      <c r="B19" s="21"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="21"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="20"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="54"/>
       <c r="G19" s="54"/>
-      <c r="H19" s="21"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="54"/>
       <c r="J19" s="54"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="21"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="20" spans="1:12" ht="12">
-      <c r="A20" s="17"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="25"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="55"/>
       <c r="G20" s="55"/>
-      <c r="H20" s="25"/>
+      <c r="H20" s="24"/>
       <c r="I20" s="55"/>
       <c r="J20" s="55"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="21"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="20"/>
     </row>
     <row r="21" spans="1:12" ht="12">
-      <c r="B21" s="31"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="57"/>
       <c r="D21" s="57"/>
-      <c r="E21" s="31"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="57"/>
       <c r="G21" s="57"/>
-      <c r="H21" s="31"/>
+      <c r="H21" s="30"/>
       <c r="I21" s="57"/>
       <c r="J21" s="57"/>
-      <c r="K21" s="31"/>
+      <c r="K21" s="30"/>
     </row>
     <row r="22" spans="1:12" ht="12">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
       <c r="F22" s="56"/>
       <c r="G22" s="56"/>
       <c r="I22" s="56"/>
@@ -2421,41 +2410,41 @@
   <dimension ref="A3:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:O5"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="4" style="18" customWidth="1"/>
-    <col min="6" max="8" width="10.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="18"/>
-    <col min="10" max="10" width="10.33203125" style="18" customWidth="1"/>
-    <col min="11" max="11" width="36.5" style="18" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" style="18" customWidth="1"/>
-    <col min="13" max="13" width="14.5" style="18" customWidth="1"/>
-    <col min="14" max="15" width="7.33203125" style="18" customWidth="1"/>
-    <col min="16" max="19" width="10.33203125" style="18" customWidth="1"/>
-    <col min="20" max="16384" width="17.1640625" style="18"/>
+    <col min="1" max="1" width="1.6640625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="17" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="4" style="17" customWidth="1"/>
+    <col min="6" max="8" width="10.33203125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="17"/>
+    <col min="10" max="10" width="10.33203125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="36.5" style="17" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="17" customWidth="1"/>
+    <col min="13" max="13" width="14.5" style="17" customWidth="1"/>
+    <col min="14" max="15" width="7.33203125" style="17" customWidth="1"/>
+    <col min="16" max="19" width="10.33203125" style="17" customWidth="1"/>
+    <col min="20" max="16384" width="17.1640625" style="17"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:15" ht="12">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="47"/>
       <c r="F3" s="47"/>
       <c r="G3" s="47"/>
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
       <c r="J3" s="47"/>
-      <c r="K3" s="19"/>
+      <c r="K3" s="18"/>
     </row>
     <row r="4" spans="1:15" ht="12">
-      <c r="A4" s="17"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="48" t="s">
         <v>0</v>
       </c>
@@ -2471,334 +2460,334 @@
       </c>
       <c r="I4" s="49"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="35" t="s">
+      <c r="L4" s="20"/>
+      <c r="M4" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="35">
+      <c r="N4" s="34">
         <v>0</v>
       </c>
-      <c r="O4" s="35">
+      <c r="O4" s="34">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="12">
-      <c r="A5" s="17"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="46" t="s">
         <v>36</v>
       </c>
       <c r="D5" s="46"/>
-      <c r="E5" s="22"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="46" t="s">
         <v>48</v>
       </c>
       <c r="G5" s="46"/>
-      <c r="H5" s="22"/>
+      <c r="H5" s="21"/>
       <c r="I5" s="46"/>
       <c r="J5" s="46"/>
       <c r="K5" s="51"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="35" t="s">
+      <c r="L5" s="20"/>
+      <c r="M5" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="N5" s="35">
+      <c r="N5" s="34">
         <v>9</v>
       </c>
-      <c r="O5" s="35">
+      <c r="O5" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="12">
-      <c r="A6" s="17"/>
-      <c r="B6" s="23" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="54" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="54"/>
-      <c r="H6" s="21"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="54"/>
       <c r="J6" s="54"/>
       <c r="K6" s="52"/>
-      <c r="L6" s="21"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:15" ht="51" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="54"/>
       <c r="G7" s="54"/>
-      <c r="H7" s="21"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="54"/>
       <c r="J7" s="54"/>
       <c r="K7" s="52"/>
-      <c r="L7" s="21"/>
+      <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:15" ht="12">
-      <c r="A8" s="17"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="55"/>
       <c r="G8" s="55"/>
-      <c r="H8" s="25"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="55"/>
       <c r="J8" s="55"/>
       <c r="K8" s="53"/>
-      <c r="L8" s="21"/>
+      <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:15" ht="12">
-      <c r="A9" s="17"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="46" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="46"/>
-      <c r="E9" s="22"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="46"/>
       <c r="G9" s="46"/>
-      <c r="H9" s="22"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="46"/>
       <c r="J9" s="46"/>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="21"/>
+      <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:15" ht="12">
-      <c r="A10" s="17"/>
-      <c r="B10" s="23" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="21"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="54"/>
       <c r="G10" s="54"/>
-      <c r="H10" s="21"/>
+      <c r="H10" s="20"/>
       <c r="I10" s="54"/>
       <c r="J10" s="54"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="21"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:15" ht="36">
-      <c r="A11" s="17"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="21"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="54"/>
       <c r="G11" s="54"/>
-      <c r="H11" s="21"/>
+      <c r="H11" s="20"/>
       <c r="I11" s="54"/>
       <c r="J11" s="54"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="21"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:15" ht="12">
-      <c r="A12" s="17"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="25"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="55"/>
       <c r="G12" s="55"/>
-      <c r="H12" s="25"/>
+      <c r="H12" s="24"/>
       <c r="I12" s="55"/>
       <c r="J12" s="55"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="21"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:15" ht="12">
-      <c r="A13" s="17"/>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="46" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="46"/>
-      <c r="E13" s="22"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="46"/>
       <c r="G13" s="46"/>
-      <c r="H13" s="22"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="46"/>
       <c r="J13" s="46"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="21"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="20"/>
     </row>
     <row r="14" spans="1:15" ht="12">
-      <c r="A14" s="17"/>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="21"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
-      <c r="H14" s="21"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="54"/>
       <c r="J14" s="54"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="21"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="20"/>
     </row>
     <row r="15" spans="1:15" ht="24">
-      <c r="A15" s="17"/>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="21"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="54" t="s">
         <v>43</v>
       </c>
       <c r="G15" s="54"/>
-      <c r="H15" s="21"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="54" t="s">
         <v>45</v>
       </c>
       <c r="J15" s="54"/>
-      <c r="K15" s="20" t="s">
+      <c r="K15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="21"/>
+      <c r="L15" s="20"/>
     </row>
     <row r="16" spans="1:15" ht="12">
-      <c r="A16" s="17"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="25"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="55"/>
       <c r="G16" s="55"/>
-      <c r="H16" s="25"/>
+      <c r="H16" s="24"/>
       <c r="I16" s="55"/>
       <c r="J16" s="55"/>
-      <c r="K16" s="28" t="s">
+      <c r="K16" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="L16" s="21"/>
+      <c r="L16" s="20"/>
     </row>
     <row r="17" spans="1:12" ht="12">
-      <c r="A17" s="17"/>
-      <c r="B17" s="22" t="s">
+      <c r="A17" s="16"/>
+      <c r="B17" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="46" t="s">
         <v>44</v>
       </c>
       <c r="D17" s="46"/>
-      <c r="E17" s="22"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="46"/>
       <c r="G17" s="46"/>
-      <c r="H17" s="22"/>
+      <c r="H17" s="21"/>
       <c r="I17" s="46"/>
       <c r="J17" s="46"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="21"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="20"/>
     </row>
     <row r="18" spans="1:12" ht="12">
-      <c r="A18" s="17"/>
-      <c r="B18" s="23" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="21"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
-      <c r="H18" s="21"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="54"/>
       <c r="J18" s="54"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="21"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="20"/>
     </row>
     <row r="19" spans="1:12" ht="48">
-      <c r="A19" s="17"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="21"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="54" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="54"/>
-      <c r="H19" s="21"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="54"/>
       <c r="J19" s="54"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="21"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="20" spans="1:12" ht="12">
-      <c r="A20" s="17"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="25"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="55"/>
       <c r="G20" s="55"/>
-      <c r="H20" s="25"/>
+      <c r="H20" s="24"/>
       <c r="I20" s="55"/>
       <c r="J20" s="55"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="21"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="20"/>
     </row>
     <row r="21" spans="1:12" ht="12">
-      <c r="B21" s="31"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="57"/>
       <c r="D21" s="57"/>
-      <c r="E21" s="31"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="57"/>
       <c r="G21" s="57"/>
-      <c r="H21" s="31"/>
+      <c r="H21" s="30"/>
       <c r="I21" s="57"/>
       <c r="J21" s="57"/>
-      <c r="K21" s="31"/>
+      <c r="K21" s="30"/>
     </row>
     <row r="22" spans="1:12" ht="12">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
       <c r="F22" s="56"/>
       <c r="G22" s="56"/>
       <c r="I22" s="56"/>

</xml_diff>